<commit_message>
HR1 case study updated.
</commit_message>
<xml_diff>
--- a/data/Simulations/HR1/Location1/Location1_2020.xlsx
+++ b/data/Simulations/HR1/Location1/Location1_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\shared-resources-planning-v3\data\Simulations\HR1\Location1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009C64C1-8AD2-4BD4-B2F2-850176CEF6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47830FE5-6CAD-4083-BAAA-EDDC58013712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="GenStatus, Winter" sheetId="4" r:id="rId6"/>
     <sheet name="DownFlex, Winter" sheetId="7" r:id="rId7"/>
     <sheet name="UpFlex, Winter" sheetId="8" r:id="rId8"/>
-    <sheet name="CostFlex" sheetId="9" r:id="rId9"/>
+    <sheet name="CostFlex, Winter" sheetId="9" r:id="rId9"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId10"/>
@@ -5013,7 +5013,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A3" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11521,7 +11521,7 @@
   <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="A1:Y15"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13860,8 +13860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974DD06D-D26C-4C05-BDC7-26713BF8A97D}">
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21476,8 +21476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A493BBFE-7EA1-4C70-88FB-3F661833D41A}">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21564,76 +21564,76 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C2" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D2" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E2" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F2" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G2" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H2" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I2" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J2" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K2" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L2" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M2" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N2" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O2" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P2" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q2" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R2" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S2" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T2" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U2" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V2" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W2" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X2" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y2" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -21641,76 +21641,76 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C3" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D3" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E3" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F3" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G3" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H3" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I3" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J3" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K3" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L3" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M3" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N3" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O3" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P3" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q3" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R3" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S3" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T3" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U3" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V3" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W3" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X3" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y3" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -21718,76 +21718,76 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C4" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D4" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E4" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F4" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G4" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H4" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I4" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J4" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K4" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L4" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M4" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N4" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O4" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P4" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q4" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R4" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S4" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T4" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U4" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V4" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W4" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X4" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y4" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -21795,76 +21795,76 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C5" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D5" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E5" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F5" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G5" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H5" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I5" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J5" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K5" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L5" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M5" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N5" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O5" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P5" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q5" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R5" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S5" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T5" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U5" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V5" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W5" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X5" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y5" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -21872,76 +21872,76 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C6" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D6" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E6" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F6" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G6" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H6" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I6" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J6" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K6" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L6" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M6" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N6" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O6" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P6" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q6" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R6" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S6" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T6" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U6" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V6" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W6" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X6" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y6" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -21949,76 +21949,76 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C7" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D7" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E7" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F7" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G7" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H7" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I7" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J7" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K7" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L7" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M7" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N7" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O7" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P7" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q7" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R7" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S7" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T7" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U7" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V7" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W7" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X7" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y7" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -22026,76 +22026,76 @@
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C8" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D8" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E8" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F8" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G8" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H8" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I8" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J8" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K8" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L8" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M8" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N8" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O8" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P8" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q8" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R8" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S8" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T8" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U8" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V8" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W8" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X8" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y8" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -22103,76 +22103,76 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C9" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D9" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E9" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F9" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G9" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H9" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I9" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J9" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K9" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L9" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M9" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N9" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O9" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P9" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q9" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R9" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S9" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T9" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U9" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V9" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W9" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X9" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y9" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -22180,76 +22180,76 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C10" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D10" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E10" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F10" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G10" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H10" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I10" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J10" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K10" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L10" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M10" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N10" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O10" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P10" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q10" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R10" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S10" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T10" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U10" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V10" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W10" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X10" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y10" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -22257,76 +22257,76 @@
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C11" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D11" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E11" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F11" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G11" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H11" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I11" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J11" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K11" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L11" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M11" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N11" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O11" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P11" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q11" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R11" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S11" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T11" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U11" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V11" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W11" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X11" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y11" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -22334,76 +22334,76 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C12" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D12" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E12" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F12" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G12" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H12" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I12" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J12" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K12" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L12" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M12" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N12" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O12" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P12" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q12" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R12" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S12" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T12" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U12" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V12" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W12" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X12" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y12" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -22411,76 +22411,76 @@
         <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C13" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D13" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E13" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F13" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G13" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H13" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I13" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J13" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K13" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L13" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M13" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N13" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O13" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P13" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q13" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R13" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S13" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T13" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U13" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V13" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W13" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X13" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y13" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -22488,76 +22488,76 @@
         <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C14" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D14" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E14" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F14" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G14" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H14" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I14" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J14" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K14" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L14" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M14" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N14" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O14" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P14" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q14" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R14" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S14" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T14" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U14" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V14" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W14" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X14" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y14" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -22565,76 +22565,76 @@
         <v>15</v>
       </c>
       <c r="B15" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C15" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D15" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E15" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F15" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G15" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H15" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I15" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J15" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K15" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L15" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M15" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N15" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O15" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P15" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q15" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R15" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S15" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T15" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U15" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V15" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W15" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X15" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y15" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -22642,76 +22642,76 @@
         <v>16</v>
       </c>
       <c r="B16" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C16" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D16" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E16" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F16" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G16" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H16" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I16" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J16" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K16" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L16" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M16" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N16" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O16" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P16" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q16" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R16" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S16" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T16" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U16" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V16" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W16" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X16" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y16" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -22719,76 +22719,76 @@
         <v>17</v>
       </c>
       <c r="B17" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C17" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D17" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E17" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F17" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G17" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H17" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I17" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J17" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K17" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L17" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M17" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N17" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O17" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P17" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q17" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R17" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S17" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T17" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U17" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V17" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W17" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X17" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y17" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -22796,76 +22796,76 @@
         <v>18</v>
       </c>
       <c r="B18" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C18" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D18" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E18" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F18" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G18" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H18" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I18" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J18" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K18" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L18" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M18" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N18" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O18" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P18" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q18" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R18" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S18" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T18" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U18" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V18" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W18" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X18" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y18" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -22873,76 +22873,76 @@
         <v>19</v>
       </c>
       <c r="B19" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C19" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D19" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E19" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F19" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G19" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H19" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I19" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J19" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K19" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L19" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M19" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N19" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O19" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P19" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q19" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R19" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S19" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T19" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U19" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V19" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W19" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X19" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y19" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -22950,76 +22950,76 @@
         <v>20</v>
       </c>
       <c r="B20" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C20" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D20" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E20" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F20" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G20" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H20" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I20" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J20" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K20" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L20" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M20" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N20" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O20" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P20" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q20" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R20" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S20" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T20" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U20" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V20" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W20" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X20" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y20" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -23027,76 +23027,76 @@
         <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C21" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D21" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E21" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F21" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G21" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H21" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I21" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J21" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K21" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L21" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M21" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N21" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O21" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P21" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q21" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R21" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S21" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T21" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U21" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V21" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W21" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X21" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y21" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -23104,76 +23104,76 @@
         <v>26</v>
       </c>
       <c r="B22" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C22" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D22" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E22" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F22" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G22" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H22" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I22" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J22" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K22" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L22" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M22" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N22" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O22" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P22" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q22" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R22" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S22" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T22" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U22" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V22" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W22" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X22" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y22" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -23181,76 +23181,76 @@
         <v>29</v>
       </c>
       <c r="B23" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C23" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D23" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E23" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F23" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G23" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H23" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I23" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J23" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K23" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L23" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M23" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N23" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O23" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P23" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q23" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R23" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S23" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T23" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U23" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V23" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W23" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X23" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y23" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -23258,76 +23258,76 @@
         <v>30</v>
       </c>
       <c r="B24" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C24" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D24" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E24" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F24" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G24" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H24" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I24" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J24" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K24" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L24" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M24" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N24" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O24" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P24" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q24" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R24" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S24" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T24" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U24" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V24" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W24" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X24" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y24" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -23335,76 +23335,76 @@
         <v>34</v>
       </c>
       <c r="B25" s="1">
-        <v>89.255110882890989</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C25" s="1">
-        <v>85.047658782374285</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D25" s="1">
-        <v>83.28251869443821</v>
+        <v>11.728</v>
       </c>
       <c r="E25" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F25" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G25" s="1">
-        <v>85.134311113963861</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H25" s="1">
-        <v>92.377804165730609</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I25" s="1">
-        <v>95.827850701242014</v>
+        <v>13.834</v>
       </c>
       <c r="J25" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K25" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L25" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M25" s="1">
-        <v>84.155460701562973</v>
+        <v>7.24</v>
       </c>
       <c r="N25" s="1">
-        <v>81.825475785487342</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O25" s="1">
-        <v>69.93164093841267</v>
+        <v>9.032</v>
       </c>
       <c r="P25" s="1">
-        <v>72.755865079110364</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q25" s="1">
-        <v>65.974517795821427</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R25" s="1">
-        <v>64.186912288584367</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S25" s="1">
-        <v>63.846721653454864</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T25" s="1">
-        <v>64.687570204435318</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U25" s="1">
-        <v>73.471549151128087</v>
+        <v>3.95</v>
       </c>
       <c r="V25" s="1">
-        <v>89.049712763567527</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W25" s="1">
-        <v>88.930966975833641</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X25" s="1">
-        <v>84.206810231393831</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y25" s="1">
-        <v>80.102057190538858</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -23412,76 +23412,76 @@
         <v>35</v>
       </c>
       <c r="B26" s="1">
-        <v>89.255110882891003</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C26" s="1">
-        <v>85.047658782374299</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D26" s="1">
-        <v>83.282518694438195</v>
+        <v>11.728</v>
       </c>
       <c r="E26" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F26" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G26" s="1">
-        <v>85.134311113963903</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H26" s="1">
-        <v>92.377804165730595</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I26" s="1">
-        <v>95.827850701241999</v>
+        <v>13.834</v>
       </c>
       <c r="J26" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K26" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L26" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M26" s="1">
-        <v>84.155460701563001</v>
+        <v>7.24</v>
       </c>
       <c r="N26" s="1">
-        <v>81.825475785487299</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O26" s="1">
-        <v>69.931640938412698</v>
+        <v>9.032</v>
       </c>
       <c r="P26" s="1">
-        <v>72.755865079110393</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q26" s="1">
-        <v>65.974517795821399</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R26" s="1">
-        <v>64.186912288584395</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S26" s="1">
-        <v>63.8467216534549</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T26" s="1">
-        <v>64.687570204435303</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U26" s="1">
-        <v>73.471549151128102</v>
+        <v>3.95</v>
       </c>
       <c r="V26" s="1">
-        <v>89.049712763567499</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W26" s="1">
-        <v>88.930966975833599</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X26" s="1">
-        <v>84.206810231393803</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y26" s="1">
-        <v>80.1020571905389</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -23489,76 +23489,76 @@
         <v>36</v>
       </c>
       <c r="B27" s="1">
-        <v>89.255110882891003</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C27" s="1">
-        <v>85.047658782374299</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D27" s="1">
-        <v>83.282518694438195</v>
+        <v>11.728</v>
       </c>
       <c r="E27" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F27" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G27" s="1">
-        <v>85.134311113963903</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H27" s="1">
-        <v>92.377804165730595</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I27" s="1">
-        <v>95.827850701241999</v>
+        <v>13.834</v>
       </c>
       <c r="J27" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K27" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L27" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M27" s="1">
-        <v>84.155460701563001</v>
+        <v>7.24</v>
       </c>
       <c r="N27" s="1">
-        <v>81.825475785487299</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O27" s="1">
-        <v>69.931640938412698</v>
+        <v>9.032</v>
       </c>
       <c r="P27" s="1">
-        <v>72.755865079110393</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q27" s="1">
-        <v>65.974517795821399</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R27" s="1">
-        <v>64.186912288584395</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S27" s="1">
-        <v>63.8467216534549</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T27" s="1">
-        <v>64.687570204435303</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U27" s="1">
-        <v>73.471549151128102</v>
+        <v>3.95</v>
       </c>
       <c r="V27" s="1">
-        <v>89.049712763567499</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W27" s="1">
-        <v>88.930966975833599</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X27" s="1">
-        <v>84.206810231393803</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y27" s="1">
-        <v>80.1020571905389</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -23566,76 +23566,76 @@
         <v>42</v>
       </c>
       <c r="B28" s="1">
-        <v>89.255110882891003</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C28" s="1">
-        <v>85.047658782374299</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D28" s="1">
-        <v>83.282518694438195</v>
+        <v>11.728</v>
       </c>
       <c r="E28" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F28" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G28" s="1">
-        <v>85.134311113963903</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H28" s="1">
-        <v>92.377804165730595</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I28" s="1">
-        <v>95.827850701241999</v>
+        <v>13.834</v>
       </c>
       <c r="J28" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K28" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L28" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M28" s="1">
-        <v>84.155460701563001</v>
+        <v>7.24</v>
       </c>
       <c r="N28" s="1">
-        <v>81.825475785487299</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O28" s="1">
-        <v>69.931640938412698</v>
+        <v>9.032</v>
       </c>
       <c r="P28" s="1">
-        <v>72.755865079110393</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q28" s="1">
-        <v>65.974517795821399</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R28" s="1">
-        <v>64.186912288584395</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S28" s="1">
-        <v>63.8467216534549</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T28" s="1">
-        <v>64.687570204435303</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U28" s="1">
-        <v>73.471549151128102</v>
+        <v>3.95</v>
       </c>
       <c r="V28" s="1">
-        <v>89.049712763567499</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W28" s="1">
-        <v>88.930966975833599</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X28" s="1">
-        <v>84.206810231393803</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y28" s="1">
-        <v>80.1020571905389</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -23643,76 +23643,76 @@
         <v>55</v>
       </c>
       <c r="B29" s="1">
-        <v>89.255110882891003</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C29" s="1">
-        <v>85.047658782374299</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D29" s="1">
-        <v>83.282518694438195</v>
+        <v>11.728</v>
       </c>
       <c r="E29" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F29" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G29" s="1">
-        <v>85.134311113963903</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H29" s="1">
-        <v>92.377804165730595</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I29" s="1">
-        <v>95.827850701241999</v>
+        <v>13.834</v>
       </c>
       <c r="J29" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K29" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L29" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M29" s="1">
-        <v>84.155460701563001</v>
+        <v>7.24</v>
       </c>
       <c r="N29" s="1">
-        <v>81.825475785487299</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O29" s="1">
-        <v>69.931640938412698</v>
+        <v>9.032</v>
       </c>
       <c r="P29" s="1">
-        <v>72.755865079110393</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q29" s="1">
-        <v>65.974517795821399</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R29" s="1">
-        <v>64.186912288584395</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S29" s="1">
-        <v>63.8467216534549</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T29" s="1">
-        <v>64.687570204435303</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U29" s="1">
-        <v>73.471549151128102</v>
+        <v>3.95</v>
       </c>
       <c r="V29" s="1">
-        <v>89.049712763567499</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W29" s="1">
-        <v>88.930966975833599</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X29" s="1">
-        <v>84.206810231393803</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y29" s="1">
-        <v>80.1020571905389</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
@@ -23720,76 +23720,76 @@
         <v>68</v>
       </c>
       <c r="B30" s="1">
-        <v>89.255110882891003</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C30" s="1">
-        <v>85.047658782374299</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D30" s="1">
-        <v>83.282518694438195</v>
+        <v>11.728</v>
       </c>
       <c r="E30" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F30" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G30" s="1">
-        <v>85.134311113963903</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H30" s="1">
-        <v>92.377804165730595</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I30" s="1">
-        <v>95.827850701241999</v>
+        <v>13.834</v>
       </c>
       <c r="J30" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K30" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L30" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M30" s="1">
-        <v>84.155460701563001</v>
+        <v>7.24</v>
       </c>
       <c r="N30" s="1">
-        <v>81.825475785487299</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O30" s="1">
-        <v>69.931640938412698</v>
+        <v>9.032</v>
       </c>
       <c r="P30" s="1">
-        <v>72.755865079110393</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q30" s="1">
-        <v>65.974517795821399</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R30" s="1">
-        <v>64.186912288584395</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S30" s="1">
-        <v>63.8467216534549</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T30" s="1">
-        <v>64.687570204435303</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U30" s="1">
-        <v>73.471549151128102</v>
+        <v>3.95</v>
       </c>
       <c r="V30" s="1">
-        <v>89.049712763567499</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W30" s="1">
-        <v>88.930966975833599</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X30" s="1">
-        <v>84.206810231393803</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y30" s="1">
-        <v>80.1020571905389</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
@@ -23797,76 +23797,76 @@
         <v>72</v>
       </c>
       <c r="B31" s="1">
-        <v>89.255110882891003</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C31" s="1">
-        <v>85.047658782374299</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D31" s="1">
-        <v>83.282518694438195</v>
+        <v>11.728</v>
       </c>
       <c r="E31" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F31" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G31" s="1">
-        <v>85.134311113963903</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H31" s="1">
-        <v>92.377804165730595</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I31" s="1">
-        <v>95.827850701241999</v>
+        <v>13.834</v>
       </c>
       <c r="J31" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K31" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L31" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M31" s="1">
-        <v>84.155460701563001</v>
+        <v>7.24</v>
       </c>
       <c r="N31" s="1">
-        <v>81.825475785487299</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O31" s="1">
-        <v>69.931640938412698</v>
+        <v>9.032</v>
       </c>
       <c r="P31" s="1">
-        <v>72.755865079110393</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q31" s="1">
-        <v>65.974517795821399</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R31" s="1">
-        <v>64.186912288584395</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S31" s="1">
-        <v>63.8467216534549</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T31" s="1">
-        <v>64.687570204435303</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U31" s="1">
-        <v>73.471549151128102</v>
+        <v>3.95</v>
       </c>
       <c r="V31" s="1">
-        <v>89.049712763567499</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W31" s="1">
-        <v>88.930966975833599</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X31" s="1">
-        <v>84.206810231393803</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y31" s="1">
-        <v>80.1020571905389</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -23874,76 +23874,76 @@
         <v>103</v>
       </c>
       <c r="B32" s="1">
-        <v>89.255110882891003</v>
+        <v>14.186000000000002</v>
       </c>
       <c r="C32" s="1">
-        <v>85.047658782374299</v>
+        <v>15.770000000000001</v>
       </c>
       <c r="D32" s="1">
-        <v>83.282518694438195</v>
+        <v>11.728</v>
       </c>
       <c r="E32" s="1">
-        <v>80.875509483616298</v>
+        <v>13.672000000000001</v>
       </c>
       <c r="F32" s="1">
-        <v>81.677845887223597</v>
+        <v>13.756</v>
       </c>
       <c r="G32" s="1">
-        <v>85.134311113963903</v>
+        <v>13.479999999999999</v>
       </c>
       <c r="H32" s="1">
-        <v>92.377804165730595</v>
+        <v>15.692000000000002</v>
       </c>
       <c r="I32" s="1">
-        <v>95.827850701241999</v>
+        <v>13.834</v>
       </c>
       <c r="J32" s="1">
-        <v>100</v>
+        <v>9.8580000000000005</v>
       </c>
       <c r="K32" s="1">
-        <v>94.813697487082393</v>
+        <v>10.110000000000001</v>
       </c>
       <c r="L32" s="1">
-        <v>92.660226579800394</v>
+        <v>7.5760000000000005</v>
       </c>
       <c r="M32" s="1">
-        <v>84.155460701563001</v>
+        <v>7.24</v>
       </c>
       <c r="N32" s="1">
-        <v>81.825475785487299</v>
+        <v>7.5180000000000007</v>
       </c>
       <c r="O32" s="1">
-        <v>69.931640938412698</v>
+        <v>9.032</v>
       </c>
       <c r="P32" s="1">
-        <v>72.755865079110393</v>
+        <v>8.2260000000000009</v>
       </c>
       <c r="Q32" s="1">
-        <v>65.974517795821399</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="R32" s="1">
-        <v>64.186912288584395</v>
+        <v>8.3099999999999987</v>
       </c>
       <c r="S32" s="1">
-        <v>63.8467216534549</v>
+        <v>7.7359999999999998</v>
       </c>
       <c r="T32" s="1">
-        <v>64.687570204435303</v>
+        <v>6.3180000000000005</v>
       </c>
       <c r="U32" s="1">
-        <v>73.471549151128102</v>
+        <v>3.95</v>
       </c>
       <c r="V32" s="1">
-        <v>89.049712763567499</v>
+        <v>4.7459999999999996</v>
       </c>
       <c r="W32" s="1">
-        <v>88.930966975833599</v>
+        <v>6.0860000000000003</v>
       </c>
       <c r="X32" s="1">
-        <v>84.206810231393803</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="Y32" s="1">
-        <v>80.1020571905389</v>
+        <v>9.6480000000000015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>